<commit_message>
learning stream sum method
</commit_message>
<xml_diff>
--- a/query/note_myo/queryNote.xlsx
+++ b/query/note_myo/queryNote.xlsx
@@ -4,16 +4,17 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17260" activeTab="3"/>
+    <workbookView windowWidth="20600" windowHeight="12520" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="class Digram" sheetId="1" r:id="rId1"/>
     <sheet name="Course Entity" sheetId="2" r:id="rId2"/>
-    <sheet name="Section Entity" sheetId="3" r:id="rId3"/>
-    <sheet name="SectionPK Entity" sheetId="4" r:id="rId4"/>
+    <sheet name="Section Entity" sheetId="7" r:id="rId3"/>
+    <sheet name="SectionPK" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'class Digram'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">SectionPK!$A$1:$K$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,6 +33,339 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="93">
+  <si>
+    <t>package com.query.entity;</t>
+  </si>
+  <si>
+    <t>Course Table</t>
+  </si>
+  <si>
+    <t>import jakarta.persistence.Entity;</t>
+  </si>
+  <si>
+    <t>import jakarta.persistence.GeneratedValue;</t>
+  </si>
+  <si>
+    <t>import jakarta.persistence.GenerationType;</t>
+  </si>
+  <si>
+    <t>import jakarta.persistence.Id;</t>
+  </si>
+  <si>
+    <t>@Entity</t>
+  </si>
+  <si>
+    <t>public class Course {</t>
+  </si>
+  <si>
+    <t>@Id</t>
+  </si>
+  <si>
+    <t>@GeneratedValue(strategy = GenerationType.IDENTITY)</t>
+  </si>
+  <si>
+    <t>private int id;</t>
+  </si>
+  <si>
+    <t>private String name;</t>
+  </si>
+  <si>
+    <t>private int hours;</t>
+  </si>
+  <si>
+    <t>private int fees;</t>
+  </si>
+  <si>
+    <t>public Course(int id, String name, int hours, int fees) {</t>
+  </si>
+  <si>
+    <t>super();</t>
+  </si>
+  <si>
+    <t>this.id = id;</t>
+  </si>
+  <si>
+    <t>this.name = name;</t>
+  </si>
+  <si>
+    <t>this.hours = hours;</t>
+  </si>
+  <si>
+    <t>this.fees = fees;</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>public int getId() {</t>
+  </si>
+  <si>
+    <t>return id;</t>
+  </si>
+  <si>
+    <t>public void setId(int id) {</t>
+  </si>
+  <si>
+    <t>public String getName() {</t>
+  </si>
+  <si>
+    <t>return name;</t>
+  </si>
+  <si>
+    <t>public void setName(String name) {</t>
+  </si>
+  <si>
+    <t>public int getHours() {</t>
+  </si>
+  <si>
+    <t>return hours;</t>
+  </si>
+  <si>
+    <t>public void setHours(int hours) {</t>
+  </si>
+  <si>
+    <t>public int getFees() {</t>
+  </si>
+  <si>
+    <t>return fees;</t>
+  </si>
+  <si>
+    <t>public void setFees(int fees) {</t>
+  </si>
+  <si>
+    <t>@Override</t>
+  </si>
+  <si>
+    <t>public String toString() {</t>
+  </si>
+  <si>
+    <t>return "Course [id=" + id + ", name=" + name + ", hours=" + hours + ", fees=" + fees + "]";</t>
+  </si>
+  <si>
+    <t>import java.time.DayOfWeek;</t>
+  </si>
+  <si>
+    <t>import java.time.LocalDate;</t>
+  </si>
+  <si>
+    <t>import java.util.List;</t>
+  </si>
+  <si>
+    <t>import jakarta.persistence.EmbeddedId;</t>
+  </si>
+  <si>
+    <t>import jakarta.persistence.JoinColumn;</t>
+  </si>
+  <si>
+    <t>import jakarta.persistence.ManyToOne;</t>
+  </si>
+  <si>
+    <t>import lombok.Data;</t>
+  </si>
+  <si>
+    <t>@Data</t>
+  </si>
+  <si>
+    <t>public class Section {</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@EmbeddedId</t>
+    </r>
+  </si>
+  <si>
+    <t>private SectionPK id;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@ManyToOne</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@JoinColumn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(name="courseId",insertable=false,updatable=false)</t>
+    </r>
+  </si>
+  <si>
+    <t>private Course course;</t>
+  </si>
+  <si>
+    <t>    </t>
+  </si>
+  <si>
+    <t>private List&lt;DayOfWeek&gt; days;</t>
+  </si>
+  <si>
+    <t>private String startTime;</t>
+  </si>
+  <si>
+    <t>private String endTime;</t>
+  </si>
+  <si>
+    <t>private LocalDate endAt;</t>
+  </si>
+  <si>
+    <t>public Section(SectionPK id, Course course, List&lt;DayOfWeek&gt; days, String startTime, String endTime, LocalDate endAt,</t>
+  </si>
+  <si>
+    <t>int fees) {</t>
+  </si>
+  <si>
+    <t>this.course = course;</t>
+  </si>
+  <si>
+    <t>this.days = days;</t>
+  </si>
+  <si>
+    <t>this.startTime = startTime;</t>
+  </si>
+  <si>
+    <t>this.endTime = endTime;</t>
+  </si>
+  <si>
+    <t>this.endAt = endAt;</t>
+  </si>
+  <si>
+    <t>public SectionPK getId() {</t>
+  </si>
+  <si>
+    <t>public void setId(SectionPK id) {</t>
+  </si>
+  <si>
+    <t>public Course getCourse() {</t>
+  </si>
+  <si>
+    <t>return course;</t>
+  </si>
+  <si>
+    <t>public void setCourse(Course course) {</t>
+  </si>
+  <si>
+    <t>public List&lt;DayOfWeek&gt; getDays() {</t>
+  </si>
+  <si>
+    <t>return days;</t>
+  </si>
+  <si>
+    <t>public void setDays(List&lt;DayOfWeek&gt; days) {</t>
+  </si>
+  <si>
+    <t>public String getStartTime() {</t>
+  </si>
+  <si>
+    <t>return startTime;</t>
+  </si>
+  <si>
+    <t>public void setStartTime(String startTime) {</t>
+  </si>
+  <si>
+    <t>public String getEndTime() {</t>
+  </si>
+  <si>
+    <t>return endTime;</t>
+  </si>
+  <si>
+    <t>public void setEndTime(String endTime) {</t>
+  </si>
+  <si>
+    <t>public LocalDate getEndAt() {</t>
+  </si>
+  <si>
+    <t>return endAt;</t>
+  </si>
+  <si>
+    <t>public void setEndAt(LocalDate endAt) {</t>
+  </si>
+  <si>
+    <t>import jakarta.persistence.Embeddable;</t>
+  </si>
+  <si>
+    <t>@Embeddable</t>
+  </si>
+  <si>
+    <t>public class SectionPK {</t>
+  </si>
+  <si>
+    <t>private int courseId;</t>
+  </si>
+  <si>
+    <t>private LocalDate startAt;</t>
+  </si>
+  <si>
+    <t>public int getCourseId() {</t>
+  </si>
+  <si>
+    <t>return courseId;</t>
+  </si>
+  <si>
+    <t>public void setCourseId(int courseId) {</t>
+  </si>
+  <si>
+    <t>this.courseId = courseId;</t>
+  </si>
+  <si>
+    <t>public LocalDate getStartAt() {</t>
+  </si>
+  <si>
+    <t>return startAt;</t>
+  </si>
+  <si>
+    <t>public void setStartAt(LocalDate startAt) {</t>
+  </si>
+  <si>
+    <t>this.startAt = startAt;</t>
+  </si>
+  <si>
+    <t>public SectionPK(int courseId, LocalDate startAt) {</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
@@ -40,9 +374,24 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -513,138 +862,147 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -965,6 +1323,1473 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>33655</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>23495</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>366395</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangles 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="765175" y="2157095"/>
+          <a:ext cx="3990340" cy="632460"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>33020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>24130</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangles 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12700" y="1526540"/>
+          <a:ext cx="734060" cy="204470"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>319405</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>732155</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>54610</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rounded Rectangular Callout 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3977005" y="160020"/>
+          <a:ext cx="3338195" cy="1388110"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -56241"/>
+            <a:gd name="adj2" fmla="val 93289"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>@Entity ,@Id annotation </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>があれば　</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Entity</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>として作成されくれます。（テーブル名は　</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Course)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>＠</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>GeneratedValue is for auto increment</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>202565</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>462280</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>177165</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9" descr="Screenshot 2025-02-09 at 17.01.33"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8091170" y="629285"/>
+          <a:ext cx="6269990" cy="2534920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>32385</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>24765</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>429260</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangles 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="32385" y="3225165"/>
+          <a:ext cx="1859915" cy="424815"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>154940</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>704215</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>32385</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rounded Rectangular Callout 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1645920" y="2288540"/>
+          <a:ext cx="4178935" cy="730885"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -56241"/>
+            <a:gd name="adj2" fmla="val 93289"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>SectionPK is @EmbeddedId </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>courseId,startAt is crate filed in the section table</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>22225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>707390</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>78105</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangles 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12700" y="3649345"/>
+          <a:ext cx="3620770" cy="695960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>130810</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>245110</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>191770</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rounded Rectangular Callout 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3788410" y="3251200"/>
+          <a:ext cx="6210300" cy="1207770"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -54131"/>
+            <a:gd name="adj2" fmla="val 40175"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>private Course course is not list so that @ManyTo one Relationship</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>@JoinColumn(name="courseId",insertable=false,updatable=false)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>@CourseId is SectionPK class of filed ,this field is not insert and update</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>we insert and update on the course Entiy table  </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1302385</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>53975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6423025" y="175260"/>
+          <a:ext cx="6485255" cy="2865755"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>212725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>398145</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57785</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangles 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12700" y="1279525"/>
+          <a:ext cx="1116965" cy="271780"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>604520</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>53975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>285115</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>142240</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rounded Rectangular Callout 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1336040" y="267335"/>
+          <a:ext cx="3338195" cy="728345"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -56241"/>
+            <a:gd name="adj2" fmla="val 93289"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>＠</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Embeddable is used for compoiste primary key</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>courseId, StartAt is composite primary key</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -1246,47 +3071,824 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="12:12">
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2">
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3">
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3">
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3">
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3">
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3">
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3">
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3">
+      <c r="C43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3">
+      <c r="C47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3">
+      <c r="C51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3">
+      <c r="C55" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3">
+      <c r="C60" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2">
+      <c r="B61" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A96"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="7" width="9" style="1"/>
+    <col min="8" max="8" width="24.8671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.1328125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T26" sqref="T26"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="2"/>
+  <cols>
+    <col min="7" max="7" width="8.8359375" customWidth="1"/>
+    <col min="8" max="8" width="35.4140625" hidden="1" customWidth="1"/>
+    <col min="9" max="11" width="9" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="3:3">
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3">
+      <c r="C22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3">
+      <c r="C26" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3">
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3">
+      <c r="C31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3">
+      <c r="C32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>